<commit_message>
roboflow model - fishing point connected
</commit_message>
<xml_diff>
--- a/documentation/Training statistics.xlsx
+++ b/documentation/Training statistics.xlsx
@@ -32,9 +32,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Model version</t>
-  </si>
-  <si>
     <t>Precision</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Training experiments - Fishing access point camera</t>
+  </si>
+  <si>
+    <t>Model</t>
   </si>
 </sst>
 </file>
@@ -210,19 +210,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -239,6 +233,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -521,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K29"/>
+  <dimension ref="B2:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,75 +536,75 @@
     <col min="9" max="9" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B4" s="4" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="4" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="6" t="s">
+    </row>
+    <row r="5" spans="2:13" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H5" s="11"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="2:13" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
         <v>46052</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1">
         <v>33</v>
@@ -628,15 +628,15 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
         <v>46052</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1">
         <v>33</v>
@@ -659,16 +659,19 @@
       <c r="K7" s="1">
         <v>0.50900000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="M7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>46057</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1">
         <v>128</v>
@@ -691,16 +694,19 @@
       <c r="K8" s="1">
         <v>0.42699999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="M8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>46059</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="1">
         <v>128</v>
@@ -724,15 +730,15 @@
         <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>46071</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1">
         <v>236</v>
@@ -756,15 +762,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>46071</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="1">
         <v>236</v>
@@ -788,7 +794,7 @@
         <v>0.46400000000000002</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -800,7 +806,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="2:11" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:13" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -812,122 +818,150 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="18" spans="2:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="13"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B20" s="3">
+        <v>46071</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1">
+        <v>88</v>
+      </c>
+      <c r="F20" s="1">
+        <v>25</v>
+      </c>
+      <c r="G20" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B20" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>5</v>
+      <c r="H20" s="1">
+        <v>301</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.82599999999999996</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="7"/>
+      <c r="B21" s="3">
+        <v>46072</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="1">
+        <v>189</v>
+      </c>
+      <c r="F21" s="1">
+        <v>72</v>
+      </c>
+      <c r="G21" s="1">
+        <v>31</v>
+      </c>
+      <c r="H21" s="1">
+        <v>704</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.88700000000000001</v>
+      </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B22" s="3">
-        <v>46071</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="1">
-        <v>88</v>
-      </c>
-      <c r="F22" s="1">
-        <v>25</v>
-      </c>
-      <c r="G22" s="1">
-        <v>12</v>
-      </c>
-      <c r="H22" s="1">
-        <v>301</v>
-      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B23" s="3"/>
-      <c r="C23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="1">
-        <v>88</v>
-      </c>
-      <c r="F23" s="1">
-        <v>25</v>
-      </c>
-      <c r="G23" s="1">
-        <v>12</v>
-      </c>
-      <c r="H23" s="1">
-        <v>301</v>
-      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -945,7 +979,7 @@
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B25" s="3"/>
+      <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -957,7 +991,7 @@
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B26" s="3"/>
+      <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -980,41 +1014,8 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B18:K18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
@@ -1024,10 +1025,19 @@
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B16:K16"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K4" r:id="rId1"/>
-    <hyperlink ref="K20" r:id="rId2"/>
+    <hyperlink ref="K18" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>

</xml_diff>